<commit_message>
changed scripts to support multiROI
</commit_message>
<xml_diff>
--- a/tests/Results_test/Results_test_touch_needle.xlsx
+++ b/tests/Results_test/Results_test_touch_needle.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>vGlut_dsx_GCaMP6f_male_fly2_touch_needle_002-stabilizedROI.tif</t>
   </si>
@@ -71,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -87,11 +87,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -101,6 +105,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22951,40 +22959,40 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>